<commit_message>
no metropolis + updated report
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Sampler</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Photon Map</t>
-  </si>
-  <si>
-    <t>Metropolis</t>
   </si>
   <si>
     <t>Adaptive</t>
@@ -131,7 +128,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -154,7 +151,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$4:$B$4</c:f>
+              <c:f>Sheet1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -175,35 +172,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$2:$F$2</c:f>
+              <c:f>Sheet1!$D$2:$E$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Path</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Photon Map</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Metropolis</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$F$4</c:f>
+              <c:f>Sheet1!$D$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2416.3000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -214,7 +205,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$5:$B$5</c:f>
+              <c:f>Sheet1!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -235,35 +226,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$2:$F$2</c:f>
+              <c:f>Sheet1!$D$2:$E$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Path</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Photon Map</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Metropolis</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$F$5</c:f>
+              <c:f>Sheet1!$D$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>64.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2341.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -274,7 +259,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$6:$B$6</c:f>
+              <c:f>Sheet1!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -295,35 +280,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$2:$F$2</c:f>
+              <c:f>Sheet1!$D$2:$E$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Path</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Photon Map</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Metropolis</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$6:$F$6</c:f>
+              <c:f>Sheet1!$D$6:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>65.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2331.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -334,7 +313,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$7:$B$7</c:f>
+              <c:f>Sheet1!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -355,35 +334,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$2:$F$2</c:f>
+              <c:f>Sheet1!$D$2:$E$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Path</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Photon Map</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Metropolis</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$F$7</c:f>
+              <c:f>Sheet1!$D$7:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>66.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2338.6999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,7 +367,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$8:$B$8</c:f>
+              <c:f>Sheet1!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -415,35 +388,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$2:$F$2</c:f>
+              <c:f>Sheet1!$D$2:$E$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Path</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Photon Map</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Metropolis</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$8:$F$8</c:f>
+              <c:f>Sheet1!$D$8:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>57.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2318.1999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -454,7 +421,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$9:$B$9</c:f>
+              <c:f>Sheet1!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -475,35 +442,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$2:$F$2</c:f>
+              <c:f>Sheet1!$D$2:$E$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Path</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Photon Map</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Metropolis</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$9:$F$9</c:f>
+              <c:f>Sheet1!$D$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>65.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3193.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -519,11 +480,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="197588648"/>
-        <c:axId val="379788680"/>
+        <c:axId val="-39733984"/>
+        <c:axId val="-39728000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="197588648"/>
+        <c:axId val="-39733984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,7 +542,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -619,10 +580,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379788680"/>
+        <c:crossAx val="-39728000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -630,7 +591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="379788680"/>
+        <c:axId val="-39728000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -707,7 +668,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -739,10 +700,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197588648"/>
+        <c:crossAx val="-39733984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -782,7 +743,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -812,7 +773,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -826,7 +787,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -889,7 +850,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -951,7 +912,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pt-PT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1048,11 +1009,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="379784760"/>
-        <c:axId val="379782408"/>
+        <c:axId val="-39727456"/>
+        <c:axId val="-39726368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="379784760"/>
+        <c:axId val="-39727456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1071,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1148,10 +1109,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379782408"/>
+        <c:crossAx val="-39726368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1159,7 +1120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="379782408"/>
+        <c:axId val="-39726368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1192,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1263,10 +1224,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379784760"/>
+        <c:crossAx val="-39727456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1304,7 +1265,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1318,7 +1279,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1356,7 +1317,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1418,7 +1379,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pt-PT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1515,11 +1476,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="379783976"/>
-        <c:axId val="379785936"/>
+        <c:axId val="-39723648"/>
+        <c:axId val="-39725280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="379783976"/>
+        <c:axId val="-39723648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1580,7 +1541,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1618,10 +1579,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379785936"/>
+        <c:crossAx val="-39725280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1629,7 +1590,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="379785936"/>
+        <c:axId val="-39725280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1704,7 +1665,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1736,10 +1697,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379783976"/>
+        <c:crossAx val="-39723648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1777,480 +1738,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="105"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="5"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Metropolis</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-PT"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$4:$B$9</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Adaptive</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Best Candidate</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Halton</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Low Discrepancy</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Random</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Stratified</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$4:$F$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="379786328"/>
-        <c:axId val="379788288"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="379786328"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Sampler</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="379788288"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="379788288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Time (s)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="379786328"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2378,12 +1866,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
-  <a:schemeClr val="accent3"/>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3391,509 +2873,6 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4488,41 +3467,11 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>490537</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4811,7 +3760,7 @@
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4840,9 +3789,6 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -4857,13 +3803,11 @@
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
@@ -4874,13 +3818,11 @@
       <c r="E4" s="2">
         <v>2416.3000000000002</v>
       </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
@@ -4891,13 +3833,11 @@
       <c r="E5" s="2">
         <v>2341.5</v>
       </c>
-      <c r="F5" s="2">
-        <v>2</v>
-      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
@@ -4908,13 +3848,11 @@
       <c r="E6" s="2">
         <v>2331.1</v>
       </c>
-      <c r="F6" s="2">
-        <v>3</v>
-      </c>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
@@ -4925,13 +3863,11 @@
       <c r="E7" s="2">
         <v>2338.6999999999998</v>
       </c>
-      <c r="F7" s="2">
-        <v>4</v>
-      </c>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>3</v>
@@ -4942,13 +3878,11 @@
       <c r="E8" s="2">
         <v>2318.1999999999998</v>
       </c>
-      <c r="F8" s="2">
-        <v>5</v>
-      </c>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>3</v>
@@ -4959,9 +3893,7 @@
       <c r="E9" s="2">
         <v>3193.1</v>
       </c>
-      <c r="F9" s="2">
-        <v>6</v>
-      </c>
+      <c r="F9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>